<commit_message>
Remove unusually low pH values
- Replace pH values 0.73 and 0.68 with NA in data processing script
- These values were outliers and likely measurement errors
- Update processed data files
- Rebuild documentation and pkgdown website
- Closes #10

🤖 Generated with [Claude Code](https://claude.ai/code)

Co-Authored-By: Claude <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/inst/extdata/postfloodintervention.xlsx
+++ b/inst/extdata/postfloodintervention.xlsx
@@ -20154,9 +20154,7 @@
       <c r="R186" t="n">
         <v>0</v>
       </c>
-      <c r="S186" t="n">
-        <v>0.73</v>
-      </c>
+      <c r="S186"/>
       <c r="T186" t="n">
         <v>29.6</v>
       </c>
@@ -28656,9 +28654,7 @@
       <c r="R280" t="n">
         <v>0.35</v>
       </c>
-      <c r="S280" t="n">
-        <v>0.68</v>
-      </c>
+      <c r="S280"/>
       <c r="T280" t="n">
         <v>28</v>
       </c>

</xml_diff>